<commit_message>
First running version. Problems with comparing datetimes with different dates.
</commit_message>
<xml_diff>
--- a/_templates/Predictive-Maintainance-Board/Audits_DE.xlsx
+++ b/_templates/Predictive-Maintainance-Board/Audits_DE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Predictive-Maintainance-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C92FDB-4A6E-E543-8AC5-B147488F191A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3E9206-CFED-514A-A5BD-1BA357898501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-54140" yWindow="-4840" windowWidth="29220" windowHeight="28240" xr2:uid="{9B8791ED-9B43-B842-A3BF-E1360AD659B4}"/>
   </bookViews>
@@ -135,10 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +457,7 @@
   <dimension ref="A1:D815"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,8 +480,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>43760</v>
+      <c r="A2" s="3">
+        <v>43791</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -493,8 +494,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>43760</v>
+      <c r="A3" s="3">
+        <v>43791</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -507,8 +508,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>43760</v>
+      <c r="A4" s="3">
+        <v>43791</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -521,8 +522,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>43760</v>
+      <c r="A5" s="3">
+        <v>43791</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -535,8 +536,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>43760</v>
+      <c r="A6" s="3">
+        <v>43791</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -549,8 +550,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>43760</v>
+      <c r="A7" s="3">
+        <v>43793</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -563,8 +564,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>43760</v>
+      <c r="A8" s="3">
+        <v>43793</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -577,8 +578,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>43761</v>
+      <c r="A9" s="3">
+        <v>43793</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -591,8 +592,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>43761</v>
+      <c r="A10" s="3">
+        <v>43795</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -605,8 +606,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>43761</v>
+      <c r="A11" s="3">
+        <v>43795</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -619,8 +620,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>43762</v>
+      <c r="A12" s="3">
+        <v>43795</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
@@ -633,8 +634,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>43762</v>
+      <c r="A13" s="3">
+        <v>43797</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -647,8 +648,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>43762</v>
+      <c r="A14" s="3">
+        <v>43802</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -661,8 +662,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>43762</v>
+      <c r="A15" s="3">
+        <v>43802</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
@@ -675,8 +676,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>43762</v>
+      <c r="A16" s="3">
+        <v>43802</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
@@ -689,8 +690,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>43762</v>
+      <c r="A17" s="3">
+        <v>43804</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
@@ -703,8 +704,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>43762</v>
+      <c r="A18" s="3">
+        <v>43804</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
@@ -717,8 +718,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>43762</v>
+      <c r="A19" s="3">
+        <v>43804</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -731,8 +732,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>43762</v>
+      <c r="A20" s="3">
+        <v>43804</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>

</xml_diff>